<commit_message>
salida de SBR - prueba #5
</commit_message>
<xml_diff>
--- a/Reglas-salidas/4/predicciones-prueba4.xlsx
+++ b/Reglas-salidas/4/predicciones-prueba4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\Github\tangente-penitente\Reglas-salidas\4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A676B2D-F6E7-46B6-A10C-A9EC74E07D3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003869C6-343B-4717-89A1-7BB441CB5B6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="503" windowWidth="22695" windowHeight="14595" firstSheet="3" activeTab="24" xr2:uid="{C418B5A3-580C-46C4-9CFE-2287BFFC6054}"/>
+    <workbookView xWindow="-98" yWindow="503" windowWidth="22695" windowHeight="14595" firstSheet="4" activeTab="17" xr2:uid="{C418B5A3-580C-46C4-9CFE-2287BFFC6054}"/>
   </bookViews>
   <sheets>
     <sheet name="17" sheetId="1" r:id="rId1"/>
@@ -2166,8 +2166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1183B17-B92D-477C-9508-C985648AAC64}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B73"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3424,7 +3424,7 @@
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B73"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12222,8 +12222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C14D3A4-5AFB-4E3E-A638-F54AF888B68F}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B73"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -15993,8 +15993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE0BA9B-2DD1-4BFC-952F-DC5F918C0CB8}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B73"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -17251,7 +17251,7 @@
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -18507,8 +18507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE53BC81-BE17-44FD-89D3-AC878C9F57D8}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B73"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -19764,8 +19764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66A9CE6-E9E1-4339-8A36-CA01A6A4BE5A}">
   <dimension ref="AG1:AK73"/>
   <sheetViews>
-    <sheetView topLeftCell="AG38" workbookViewId="0">
-      <selection activeCell="AH2" sqref="AH2:AH73"/>
+    <sheetView topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1:AH1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -21021,8 +21021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95AE472C-40C7-4E50-BC77-730F7257F5A1}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C38" sqref="C1:C1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -22278,8 +22278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F06335B-9063-4924-A398-B19538042F1C}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -23535,8 +23535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E57D57F6-1620-43C5-AB25-726D0DE4DFB7}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B73"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -24792,8 +24792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E054D87-55C6-4A26-BE0C-F3D712B230B2}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B73"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -26049,7 +26049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74EC6EAC-3FE8-40BC-AE6C-44D264959021}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B73"/>
     </sheetView>
   </sheetViews>

</xml_diff>